<commit_message>
Change the initial-passwords.xlsx template to remove the email column
</commit_message>
<xml_diff>
--- a/static-src/initial-passwords.xlsx
+++ b/static-src/initial-passwords.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">{{firstname}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{lastname}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{email}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{login}}</t>
@@ -142,15 +139,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="19.8418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -166,9 +163,6 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>